<commit_message>
ajout graph sep gc
</commit_message>
<xml_diff>
--- a/hlm2021_nb/log.xlsx
+++ b/hlm2021_nb/log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbr/Documents/GitHub/r-projects/hlm2021_nb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5C0F81-849F-8341-9C13-91F8C13C4A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11699BCC-78BD-2F4A-8DC6-E967989BA5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2840" windowWidth="28040" windowHeight="17440" xr2:uid="{CBB7D528-5268-3746-9063-92B22DC5A056}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16400" xr2:uid="{CBB7D528-5268-3746-9063-92B22DC5A056}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
   <si>
     <t>classe</t>
   </si>
@@ -81,9 +81,6 @@
     <t>solo</t>
   </si>
   <si>
-    <t>7H8H</t>
-  </si>
-  <si>
     <t>Haut-Lac</t>
   </si>
   <si>
@@ -211,13 +208,115 @@
   </si>
   <si>
     <t>marina.claquin@edu.vs.ch</t>
+  </si>
+  <si>
+    <t>7-8H</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>123i15</t>
+  </si>
+  <si>
+    <t>123i25</t>
+  </si>
+  <si>
+    <t>rene.wyssen@edu.vs.ch</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>123j15</t>
+  </si>
+  <si>
+    <t>123j25</t>
+  </si>
+  <si>
+    <t>nicole.mottier@edu.vs.ch</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>1H</t>
+  </si>
+  <si>
+    <t>123k15</t>
+  </si>
+  <si>
+    <t>123k25</t>
+  </si>
+  <si>
+    <t>ines.martenet@edu.vs.ch</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>duo</t>
+  </si>
+  <si>
+    <t>123l15</t>
+  </si>
+  <si>
+    <t>123l25</t>
+  </si>
+  <si>
+    <t>christel.jacquier@edu.vs.ch</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>3-4H</t>
+  </si>
+  <si>
+    <t>123m15</t>
+  </si>
+  <si>
+    <t>123m25</t>
+  </si>
+  <si>
+    <t>Aline Lemasson</t>
+  </si>
+  <si>
+    <t>marie-jose.fontana@edhl.ch</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>1-2H</t>
+  </si>
+  <si>
+    <t>123n15</t>
+  </si>
+  <si>
+    <t>Mélanie Tissières</t>
+  </si>
+  <si>
+    <t>melanie.tissieres@edhl.ch</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>123p15</t>
+  </si>
+  <si>
+    <t>123p25</t>
+  </si>
+  <si>
+    <t>marine.jornod@edhl.ch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,13 +333,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -248,7 +340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,7 +350,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -276,16 +374,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -779,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B6C81A-C600-D54E-BFE2-401C83CB6896}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,178 +933,174 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="4">
+        <v>44455</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2">
+      <c r="K2" s="4">
         <v>44455</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" s="2">
-        <v>44455</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="3">
+        <v>44469</v>
+      </c>
+      <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="4">
+      <c r="K3" s="3">
         <v>44469</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="K3" s="4">
-        <v>44469</v>
-      </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="3">
+        <v>44469</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="3">
+        <v>44469</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="I4" s="4">
-        <v>44469</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="4">
-        <v>44469</v>
-      </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="6">
+        <v>44475</v>
+      </c>
+      <c r="J5" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="5">
+      <c r="K5" s="6">
         <v>44475</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="K5" s="5">
-        <v>44475</v>
-      </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="7" t="str">
@@ -1012,150 +1108,416 @@
         <v>123e15</v>
       </c>
       <c r="H6" s="7" t="str">
-        <f>"123e15"</f>
-        <v>123e15</v>
-      </c>
-      <c r="I6" s="5">
+        <f>"123e25"</f>
+        <v>123e25</v>
+      </c>
+      <c r="I6" s="6">
         <v>44475</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>37</v>
+      <c r="J6" t="s">
+        <v>36</v>
       </c>
       <c r="K6" s="8">
         <v>44475</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="6" t="s">
-        <v>41</v>
+      <c r="M6" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="6">
+        <v>44475</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="6">
+        <v>44475</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="I7" s="5">
-        <v>44475</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" s="5">
-        <v>44475</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="1">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="1">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="6">
+        <v>44475</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="6">
+        <v>44475</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="I8" s="5">
-        <v>44475</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="5">
-        <v>44475</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="3">
+        <v>44482</v>
+      </c>
+      <c r="J9" t="s">
         <v>56</v>
-      </c>
-      <c r="I9" s="4">
-        <v>44482</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="K9" s="8">
         <v>44494</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="3" t="s">
-        <v>58</v>
+      <c r="M9" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="6">
+        <v>44502</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" s="6">
+        <v>44504</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="6">
+        <v>44502</v>
+      </c>
+      <c r="J11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="6">
+        <v>44504</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="6">
+        <v>44502</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="6">
+        <v>44504</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="6">
+        <v>44502</v>
+      </c>
+      <c r="J13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="6">
+        <v>44508</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" t="s">
+        <v>80</v>
+      </c>
+      <c r="I14" s="6">
+        <v>44504</v>
+      </c>
+      <c r="J14" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="6">
+        <v>44504</v>
+      </c>
+      <c r="M14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I15" s="6">
+        <v>44525</v>
+      </c>
+      <c r="J15" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15" s="6">
+        <v>44525</v>
+      </c>
+      <c r="M15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="6">
+        <v>44536</v>
+      </c>
+      <c r="J16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K16" s="6">
+        <v>44536</v>
+      </c>
+      <c r="M16" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" display="mailto:axel.vuadens@edu.vs.ch" xr:uid="{45D1BBF5-15AF-AD4F-A3AF-F5BA47594DDD}"/>
-    <hyperlink ref="M3" r:id="rId2" display="mailto:arta.citaku@edu.vs.ch" xr:uid="{F5F9CC8B-5342-7A4D-97ED-4AFF2ACEB046}"/>
-    <hyperlink ref="M4" r:id="rId3" display="mailto:sandra.rico@edu.vs.ch" xr:uid="{3167F030-DC65-2641-A2A7-CC48A5F4685B}"/>
-    <hyperlink ref="M7" r:id="rId4" display="mailto:morgane.trutet@edu.vs.ch" xr:uid="{A983DADF-B3C3-704E-9FA0-F6830F504C05}"/>
-    <hyperlink ref="M9" r:id="rId5" display="mailto:marina.claquin@edu.vs.ch" xr:uid="{B7EDCA9A-495F-8645-BFFF-F6D8B9587702}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{FBE11EEA-ED57-0B4A-A098-5C29A3E93C33}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{B9B530C8-AFF0-AB4C-A00B-BFE7FDD7941D}"/>
+    <hyperlink ref="M4" r:id="rId3" xr:uid="{26A6F5DB-D62B-C940-8FA3-013E1D42305B}"/>
+    <hyperlink ref="M7" r:id="rId4" xr:uid="{780047C2-4422-C34F-B196-06C44AEE37E7}"/>
+    <hyperlink ref="M9" r:id="rId5" xr:uid="{F297981B-112A-E24D-B3B7-671201FC557D}"/>
+    <hyperlink ref="M10" r:id="rId6" xr:uid="{5D255517-E1E5-304C-8B3E-22B3BE6803EF}"/>
+    <hyperlink ref="M11" r:id="rId7" xr:uid="{A7826371-64B1-214B-AA07-C0149DE4696E}"/>
+    <hyperlink ref="M12" r:id="rId8" xr:uid="{2DDE8FC4-4691-A84F-A77E-513F77082940}"/>
+    <hyperlink ref="M13" r:id="rId9" xr:uid="{4E666EA7-9D43-894B-B16B-C5844555D6CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1312,18 +1674,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1345,18 +1707,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80F5AD26-E6AD-4B0E-BF9F-3ABB5D3BA5CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D652176-1426-4B90-A421-57939E43BAB7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80F5AD26-E6AD-4B0E-BF9F-3ABB5D3BA5CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>